<commit_message>
Bump version; work towards pH calibration
For release with pH fix https://github.com/EnviroDIY/YosemitechModbus/commit/574a31ce8a3755ce501438fd46fbc67808124c1b
Added work towards pH calibration in Excel #16
</commit_message>
<xml_diff>
--- a/utilities/CalibrationProtocolSpreadsheet/ph_calibration+AKA.xlsx
+++ b/utilities/CalibrationProtocolSpreadsheet/ph_calibration+AKA.xlsx
@@ -1,31 +1,41 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10309"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aaufdenkampe/Documents/Arduino/YosemitechModbus/utilities/CalibrationProtocolSpreadsheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0308B6F0-861B-3841-A336-D6C9535CC396}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{211D4E27-4B32-FF4C-9DEE-70862B2C3ABA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="23300" windowHeight="19120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10440" yWindow="460" windowWidth="23300" windowHeight="19120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="YL0918071001" sheetId="3" r:id="rId1"/>
+    <sheet name="pH-Calibration-Calcs" sheetId="1" r:id="rId2"/>
+    <sheet name="Background-Info" sheetId="2" r:id="rId3"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId4"/>
+  </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="100">
   <si>
     <t>pH</t>
   </si>
@@ -1255,15 +1265,115 @@
   </si>
   <si>
     <t>https://www.coleparmer.com/tech-article/how-to-store-clean-and-recondition-ph-electrodes</t>
+  </si>
+  <si>
+    <t>Water with UNKNOWN pH</t>
+  </si>
+  <si>
+    <t>K1-K3:</t>
+  </si>
+  <si>
+    <t>K4:K6</t>
+  </si>
+  <si>
+    <t>mean:</t>
+  </si>
+  <si>
+    <t>stdev:</t>
+  </si>
+  <si>
+    <t>Reference</t>
+  </si>
+  <si>
+    <t>tap water</t>
+  </si>
+  <si>
+    <t>µS/cm</t>
+  </si>
+  <si>
+    <t>Measured</t>
+  </si>
+  <si>
+    <t>Average</t>
+  </si>
+  <si>
+    <t>Std</t>
+  </si>
+  <si>
+    <t>%CV</t>
+  </si>
+  <si>
+    <t>Date:</t>
+  </si>
+  <si>
+    <t>mS/cm</t>
+  </si>
+  <si>
+    <t>°C</t>
+  </si>
+  <si>
+    <t>SN:</t>
+  </si>
+  <si>
+    <t>YL0918071001</t>
+  </si>
+  <si>
+    <t>Version:</t>
+  </si>
+  <si>
+    <t>hw 1.2,sw 1.8</t>
+  </si>
+  <si>
+    <t>Set User Coefficients to:</t>
+  </si>
+  <si>
+    <t>K:</t>
+  </si>
+  <si>
+    <t>B:</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>predicted</t>
+  </si>
+  <si>
+    <t>residual</t>
+  </si>
+  <si>
+    <t>previous</t>
+  </si>
+  <si>
+    <t>slope</t>
+  </si>
+  <si>
+    <t>intercept</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <numFmts count="4">
+    <numFmt numFmtId="164" formatCode="0.0000"/>
+    <numFmt numFmtId="165" formatCode="0.000000"/>
+    <numFmt numFmtId="166" formatCode="0.00000"/>
+    <numFmt numFmtId="167" formatCode="yyyy\-mm\-dd"/>
+  </numFmts>
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -1317,13 +1427,56 @@
       <name val="Lucida Grande"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF0070C0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -1335,21 +1488,56 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="2" applyFill="1"/>
+    <xf numFmtId="2" fontId="12" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="12" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="12" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="10" fontId="12" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="167" fontId="1" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="1" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="4">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="2" xr:uid="{821B4227-63BD-8D4E-BB2A-3848E5F4C2AF}"/>
+    <cellStyle name="Percent 2" xfId="3" xr:uid="{07F2656E-E2C5-164B-A227-F5043B673540}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1365,6 +1553,787 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1100" b="1" i="0" u="none" strike="noStrike" baseline="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Arial"/>
+                <a:ea typeface="Arial"/>
+                <a:cs typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Calibration Curve</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.21831013640900501"/>
+          <c:y val="1.9047619047619001E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="25400">
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.17253543374775701"/>
+          <c:y val="0.104761843865186"/>
+          <c:w val="0.77817001751539305"/>
+          <c:h val="0.70952339708693901"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>References</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="diamond"/>
+            <c:size val="7"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="DD0806"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:srgbClr val="DD0806"/>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:name>linear fit</c:name>
+            <c:spPr>
+              <a:ln w="3175">
+                <a:solidFill>
+                  <a:srgbClr val="003366"/>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.42062094569784997"/>
+                  <c:y val="3.0056848275131529E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="0.000000" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln w="25400">
+                  <a:noFill/>
+                </a:ln>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                      <a:solidFill>
+                        <a:srgbClr val="000000"/>
+                      </a:solidFill>
+                      <a:latin typeface="Arial"/>
+                      <a:ea typeface="Arial"/>
+                      <a:cs typeface="Arial"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>YL0918071001!$C$22:$C$28</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>522.04683333333321</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>53.739000000000004</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-172.47499999999997</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-402.16200000000009</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>YL0918071001!$D$22:$D$28</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-CB0A-EC4A-9D9D-FF8D51961E31}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="-2133558904"/>
+        <c:axId val="-2133566584"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="-2133558904"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Arial"/>
+                    <a:ea typeface="Arial"/>
+                    <a:cs typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Measured Values</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.36267661084617903"/>
+              <c:y val="0.904761529808774"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln w="25400">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="0" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="3175">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:prstDash val="solid"/>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="0" vert="horz"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Arial"/>
+                <a:ea typeface="Arial"/>
+                <a:cs typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2133566584"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="-2133566584"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Arial"/>
+                    <a:ea typeface="Arial"/>
+                    <a:cs typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Reference Values</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="2.8169014084507001E-2"/>
+              <c:y val="0.314285714285714"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln w="25400">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="#,##0" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="3175">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:prstDash val="solid"/>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="0" vert="horz"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Arial"/>
+                <a:ea typeface="Arial"/>
+                <a:cs typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2133558904"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="25400">
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="FFFFFF"/>
+    </a:solidFill>
+    <a:ln w="3175">
+      <a:solidFill>
+        <a:srgbClr val="000000"/>
+      </a:solidFill>
+      <a:prstDash val="solid"/>
+    </a:ln>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:latin typeface="Arial"/>
+          <a:ea typeface="Arial"/>
+          <a:cs typeface="Arial"/>
+        </a:defRPr>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1" l="0.75" r="0.75" t="1" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1100" b="1" i="0" u="none" strike="noStrike" baseline="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Arial"/>
+                <a:ea typeface="Arial"/>
+                <a:cs typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Calibration Curvature</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.21428599550056199"/>
+          <c:y val="3.3898305084745797E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="25400">
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.16974708331615615"/>
+          <c:y val="0.169492226778613"/>
+          <c:w val="0.77049511481221911"/>
+          <c:h val="0.669494295775522"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Standards</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="diamond"/>
+            <c:size val="7"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="DD0806"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:srgbClr val="DD0806"/>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="3175">
+                <a:solidFill>
+                  <a:srgbClr val="000090"/>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </c:spPr>
+            <c:trendlineType val="poly"/>
+            <c:order val="2"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>YL0918071001!$C$22:$C$28</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>522.04683333333321</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>53.739000000000004</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-172.47499999999997</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-402.16200000000009</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>YL0918071001!$G$22:$G$28</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>-2.1630725649881697</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.6529542141102525</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-0.53183553036978992</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-1.958046118752236</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-4FE3-F143-995A-AA0AD5F8D523}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="-2092785320"/>
+        <c:axId val="-2092779288"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="-2092785320"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Arial"/>
+                    <a:ea typeface="Arial"/>
+                    <a:cs typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t>Measured Values</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.34642913385826801"/>
+              <c:y val="0.83051181102362204"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln w="25400">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="0" sourceLinked="0"/>
+        <c:majorTickMark val="cross"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="3175">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:prstDash val="solid"/>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="0" vert="horz"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Arial"/>
+                <a:ea typeface="Arial"/>
+                <a:cs typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2092779288"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="-2092779288"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Arial"/>
+                    <a:ea typeface="Arial"/>
+                    <a:cs typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Residual</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="2.8571428571428598E-2"/>
+              <c:y val="0.29661150407046599"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln w="25400">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="#,##0.00" sourceLinked="0"/>
+        <c:majorTickMark val="cross"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="3175">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:prstDash val="solid"/>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="0" vert="horz"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Arial"/>
+                <a:ea typeface="Arial"/>
+                <a:cs typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2092785320"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="25400">
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="FFFFFF"/>
+    </a:solidFill>
+    <a:ln w="3175">
+      <a:solidFill>
+        <a:srgbClr val="000000"/>
+      </a:solidFill>
+      <a:prstDash val="solid"/>
+    </a:ln>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:latin typeface="Arial"/>
+          <a:ea typeface="Arial"/>
+          <a:cs typeface="Arial"/>
+        </a:defRPr>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1" l="0.75" r="0.75" t="1" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -1418,7 +2387,7 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:spPr>
-            <a:ln w="19050" cap="rnd">
+            <a:ln w="25400" cap="rnd">
               <a:noFill/>
               <a:round/>
             </a:ln>
@@ -1441,102 +2410,17 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$J$13:$J$26</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="14"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>13</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>14</c:v>
-                </c:pt>
-              </c:numCache>
+              <c:f>'pH-Calibration-Calcs'!#REF!</c:f>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$L$13:$L$26</c:f>
+              <c:f>'pH-Calibration-Calcs'!#REF!</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="14"/>
+                <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>1342.86</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>285.70999999999998</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>228.57</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>171.43</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>114.29</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>57.14</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>-57.14</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>-114.29</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>-171.43</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>-228.57</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>-285.70999999999998</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>-342.86</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>-400</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1544,7 +2428,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-0AB7-6C4C-ADA6-A40F03AA62B4}"/>
+              <c16:uniqueId val="{00000000-3FEF-E84B-A94E-D7E003791918}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1575,7 +2459,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$3:$A$12</c:f>
+              <c:f>'pH-Calibration-Calcs'!$N$9:$N$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -1614,7 +2498,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$3:$B$12</c:f>
+              <c:f>'pH-Calibration-Calcs'!$O$9:$O$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -1654,7 +2538,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-0AB7-6C4C-ADA6-A40F03AA62B4}"/>
+              <c16:uniqueId val="{00000001-3FEF-E84B-A94E-D7E003791918}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2405,13 +3289,94 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>105833</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>31750</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>118533</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>48684</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3006ECB9-2E26-2D4C-B635-D55CDAD62BD7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>127000</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>116418</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>88900</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>6351</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A2840E8E-764D-114F-971D-DC7FE8BED526}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
       <xdr:colOff>628650</xdr:colOff>
       <xdr:row>10</xdr:row>
       <xdr:rowOff>44450</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
+      <xdr:col>10</xdr:col>
       <xdr:colOff>488950</xdr:colOff>
       <xdr:row>24</xdr:row>
       <xdr:rowOff>165100</xdr:rowOff>
@@ -2421,11 +3386,13 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D9F9DDDF-963D-5544-A6F0-4FF71EF52676}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9B453A7D-8120-1444-950A-3A8C70801F53}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -2440,6 +3407,72 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="YL0916112101"/>
+      <sheetName val="YL0918071002"/>
+      <sheetName val="YL0918071005"/>
+      <sheetName val="YL0918071003"/>
+      <sheetName val="YL0918071001"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="1" refreshError="1"/>
+      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="3" refreshError="1"/>
+      <sheetData sheetId="4">
+        <row r="22">
+          <cell r="C22">
+            <v>522.04683333333321</v>
+          </cell>
+          <cell r="D22">
+            <v>1000</v>
+          </cell>
+          <cell r="G22">
+            <v>-2.1630725649881697</v>
+          </cell>
+        </row>
+        <row r="23">
+          <cell r="C23">
+            <v>53.739000000000004</v>
+          </cell>
+          <cell r="D23">
+            <v>500</v>
+          </cell>
+          <cell r="G23">
+            <v>4.6529542141102525</v>
+          </cell>
+        </row>
+        <row r="24">
+          <cell r="C24">
+            <v>-172.47499999999997</v>
+          </cell>
+          <cell r="D24">
+            <v>250</v>
+          </cell>
+          <cell r="G24">
+            <v>-0.53183553036978992</v>
+          </cell>
+        </row>
+        <row r="25">
+          <cell r="C25">
+            <v>-402.16200000000009</v>
+          </cell>
+          <cell r="D25">
+            <v>0</v>
+          </cell>
+          <cell r="G25">
+            <v>-1.958046118752236</v>
+          </cell>
+        </row>
+      </sheetData>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2738,612 +3771,1620 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F70D3772-1C70-E94B-8CD8-51A5B39099D6}">
+  <dimension ref="A1:P53"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="10.83203125" style="11" customWidth="1"/>
+    <col min="2" max="2" width="14.5" style="11" customWidth="1"/>
+    <col min="3" max="4" width="10.83203125" style="11"/>
+    <col min="5" max="5" width="3.33203125" style="11" customWidth="1"/>
+    <col min="6" max="7" width="10.83203125" style="11"/>
+    <col min="8" max="8" width="3.33203125" style="11" customWidth="1"/>
+    <col min="9" max="10" width="10.83203125" style="11"/>
+    <col min="11" max="11" width="3.33203125" style="11" customWidth="1"/>
+    <col min="12" max="13" width="10.83203125" style="11"/>
+    <col min="14" max="14" width="3.33203125" style="11" customWidth="1"/>
+    <col min="15" max="16384" width="10.83203125" style="11"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="B1" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="F1" s="12">
+        <v>1000</v>
+      </c>
+      <c r="G1" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="I1" s="12">
+        <v>500</v>
+      </c>
+      <c r="J1" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="L1" s="12">
+        <v>250</v>
+      </c>
+      <c r="M1" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="O1" s="12">
+        <v>0</v>
+      </c>
+      <c r="P1" s="11" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="B2" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="C2" s="13" t="e">
+        <f>C4*1000</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="F2" s="13">
+        <f>F4*1000</f>
+        <v>522.04683333333321</v>
+      </c>
+      <c r="G2" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="I2" s="13">
+        <f>I4*1000</f>
+        <v>53.739000000000004</v>
+      </c>
+      <c r="J2" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="L2" s="13">
+        <f>L4*1000</f>
+        <v>-172.47499999999997</v>
+      </c>
+      <c r="M2" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="O2" s="13">
+        <f>O4*1000</f>
+        <v>-402.16200000000009</v>
+      </c>
+      <c r="P2" s="11" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="F3" s="14">
+        <f>F1/F2</f>
+        <v>1.9155369521444601</v>
+      </c>
+      <c r="I3" s="14">
+        <f>I1/I2</f>
+        <v>9.3042297028229033</v>
+      </c>
+      <c r="L3" s="14">
+        <f>L1/L2</f>
+        <v>-1.449485432671402</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="B4" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="C4" s="15" t="e">
+        <f>AVERAGE(C9:C18)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D4" s="16" t="e">
+        <f>AVERAGE(D9:D18)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F4" s="15">
+        <f>AVERAGE(F9:F18)</f>
+        <v>0.52204683333333324</v>
+      </c>
+      <c r="G4" s="16">
+        <f>AVERAGE(G9:G18)</f>
+        <v>22.376149999999999</v>
+      </c>
+      <c r="I4" s="15">
+        <f>AVERAGE(I9:I18)</f>
+        <v>5.3739000000000002E-2</v>
+      </c>
+      <c r="J4" s="16">
+        <f>AVERAGE(J9:J18)</f>
+        <v>22.279583333333335</v>
+      </c>
+      <c r="L4" s="15">
+        <f>AVERAGE(L9:L18)</f>
+        <v>-0.17247499999999996</v>
+      </c>
+      <c r="M4" s="16">
+        <f>AVERAGE(M9:M18)</f>
+        <v>22.153949999999998</v>
+      </c>
+      <c r="O4" s="15">
+        <f>AVERAGE(O9:O18)</f>
+        <v>-0.40216200000000007</v>
+      </c>
+      <c r="P4" s="16">
+        <f>AVERAGE(P9:P18)</f>
+        <v>22.111216666666664</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="B5" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="C5" s="15" t="e">
+        <f>STDEV(C9:C18)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D5" s="16" t="e">
+        <f>STDEV(D9:D18)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F5" s="15">
+        <f>STDEV(F9:F18)</f>
+        <v>7.0290068051371798E-4</v>
+      </c>
+      <c r="G5" s="16">
+        <f>STDEV(G9:G18)</f>
+        <v>1.6354379230040753E-2</v>
+      </c>
+      <c r="I5" s="15">
+        <f>STDEV(I9:I18)</f>
+        <v>1.5044866234034863E-4</v>
+      </c>
+      <c r="J5" s="16">
+        <f>STDEV(J9:J18)</f>
+        <v>1.6244394315168918E-2</v>
+      </c>
+      <c r="L5" s="15">
+        <f>STDEV(L9:L18)</f>
+        <v>7.3804119126238119E-4</v>
+      </c>
+      <c r="M5" s="16">
+        <f>STDEV(M9:M18)</f>
+        <v>1.7193432467078516E-2</v>
+      </c>
+      <c r="O5" s="15">
+        <f>STDEV(O9:O18)</f>
+        <v>1.3923361663046067E-4</v>
+      </c>
+      <c r="P5" s="16">
+        <f>STDEV(P9:P18)</f>
+        <v>7.8398205761779898E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="B6" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="C6" s="17" t="e">
+        <f>C5/C4</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D6" s="17" t="e">
+        <f>D5/D4</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F6" s="17">
+        <f>F5/F4</f>
+        <v>1.3464322272115142E-3</v>
+      </c>
+      <c r="G6" s="17">
+        <f>G5/G4</f>
+        <v>7.3088441175272567E-4</v>
+      </c>
+      <c r="I6" s="17">
+        <f>I5/I4</f>
+        <v>2.7996178257940906E-3</v>
+      </c>
+      <c r="J6" s="17">
+        <f>J5/J4</f>
+        <v>7.2911571424520585E-4</v>
+      </c>
+      <c r="L6" s="17">
+        <f>L5/L4</f>
+        <v>-4.279119821785078E-3</v>
+      </c>
+      <c r="M6" s="17">
+        <f>M5/M4</f>
+        <v>7.7608879983382274E-4</v>
+      </c>
+      <c r="O6" s="17">
+        <f>O5/O4</f>
+        <v>-3.4621276159970522E-4</v>
+      </c>
+      <c r="P6" s="17">
+        <f>P5/P4</f>
+        <v>3.5456305703868206E-4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A8" s="18" t="s">
+        <v>83</v>
+      </c>
+      <c r="B8" s="19">
+        <v>43368</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="F8" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="G8" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="I8" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="J8" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="L8" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="M8" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="O8" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="P8" s="11" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A9" s="18" t="s">
+        <v>86</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="C9" s="20"/>
+      <c r="D9" s="21"/>
+      <c r="F9" s="12">
+        <v>0.52095400000000003</v>
+      </c>
+      <c r="G9" s="12">
+        <v>22.38861</v>
+      </c>
+      <c r="I9" s="12">
+        <v>5.3568999999999999E-2</v>
+      </c>
+      <c r="J9" s="12">
+        <v>22.28107</v>
+      </c>
+      <c r="L9" s="12">
+        <v>-0.17135400000000001</v>
+      </c>
+      <c r="M9" s="12">
+        <v>22.168849999999999</v>
+      </c>
+      <c r="O9" s="12">
+        <v>-0.40223300000000001</v>
+      </c>
+      <c r="P9" s="12">
+        <v>22.109739999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A10" s="18" t="s">
+        <v>88</v>
+      </c>
+      <c r="B10" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="C10" s="20"/>
+      <c r="D10" s="21"/>
+      <c r="F10" s="12">
+        <v>0.52161599999999997</v>
+      </c>
+      <c r="G10" s="12">
+        <v>22.354430000000001</v>
+      </c>
+      <c r="I10" s="12">
+        <v>5.3575999999999999E-2</v>
+      </c>
+      <c r="J10" s="12">
+        <v>22.246949999999998</v>
+      </c>
+      <c r="L10" s="12">
+        <v>-0.171793</v>
+      </c>
+      <c r="M10" s="12">
+        <v>22.14743</v>
+      </c>
+      <c r="O10" s="12">
+        <v>-0.402258</v>
+      </c>
+      <c r="P10" s="12">
+        <v>22.11478</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A11" s="18"/>
+      <c r="C11" s="20"/>
+      <c r="D11" s="21"/>
+      <c r="F11" s="12">
+        <v>0.52195899999999995</v>
+      </c>
+      <c r="G11" s="12">
+        <v>22.379729999999999</v>
+      </c>
+      <c r="I11" s="12">
+        <v>5.3719000000000003E-2</v>
+      </c>
+      <c r="J11" s="12">
+        <v>22.28482</v>
+      </c>
+      <c r="L11" s="12">
+        <v>-0.173286</v>
+      </c>
+      <c r="M11" s="12">
+        <v>22.138639999999999</v>
+      </c>
+      <c r="O11" s="12">
+        <v>-0.402198</v>
+      </c>
+      <c r="P11" s="12">
+        <v>22.100950000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="C12" s="20"/>
+      <c r="D12" s="21"/>
+      <c r="F12" s="12">
+        <v>0.52224099999999996</v>
+      </c>
+      <c r="G12" s="12">
+        <v>22.380980000000001</v>
+      </c>
+      <c r="I12" s="12">
+        <v>5.3754999999999997E-2</v>
+      </c>
+      <c r="J12" s="12">
+        <v>22.288640000000001</v>
+      </c>
+      <c r="L12" s="12">
+        <v>-0.17275399999999999</v>
+      </c>
+      <c r="M12" s="12">
+        <v>22.14114</v>
+      </c>
+      <c r="O12" s="12">
+        <v>-0.402198</v>
+      </c>
+      <c r="P12" s="12">
+        <v>22.11853</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A13" s="22" t="s">
+        <v>90</v>
+      </c>
+      <c r="C13" s="20"/>
+      <c r="D13" s="21"/>
+      <c r="F13" s="12">
+        <v>0.52261299999999999</v>
+      </c>
+      <c r="G13" s="12">
+        <v>22.394929999999999</v>
+      </c>
+      <c r="I13" s="12">
+        <v>5.3919000000000002E-2</v>
+      </c>
+      <c r="J13" s="12">
+        <v>22.287379999999999</v>
+      </c>
+      <c r="L13" s="12">
+        <v>-0.17275399999999999</v>
+      </c>
+      <c r="M13" s="12">
+        <v>22.181429999999999</v>
+      </c>
+      <c r="O13" s="12">
+        <v>-0.40220299999999998</v>
+      </c>
+      <c r="P13" s="12">
+        <v>22.103490000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A14" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="B14" s="23">
+        <v>1</v>
+      </c>
+      <c r="C14" s="20"/>
+      <c r="D14" s="21"/>
+      <c r="F14" s="12">
+        <v>0.52289799999999997</v>
+      </c>
+      <c r="G14" s="12">
+        <v>22.358219999999999</v>
+      </c>
+      <c r="I14" s="12">
+        <v>5.3895999999999999E-2</v>
+      </c>
+      <c r="J14" s="12">
+        <v>22.288640000000001</v>
+      </c>
+      <c r="L14" s="12">
+        <v>-0.17290900000000001</v>
+      </c>
+      <c r="M14" s="12">
+        <v>22.14621</v>
+      </c>
+      <c r="O14" s="12">
+        <v>-0.40188200000000002</v>
+      </c>
+      <c r="P14" s="12">
+        <v>22.119810000000001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A15" s="18" t="s">
+        <v>92</v>
+      </c>
+      <c r="B15" s="23">
+        <v>0</v>
+      </c>
+      <c r="C15" s="20"/>
+      <c r="D15" s="21"/>
+      <c r="F15" s="12"/>
+      <c r="G15" s="12"/>
+      <c r="I15" s="12"/>
+      <c r="J15" s="12"/>
+      <c r="L15" s="12"/>
+      <c r="M15" s="12"/>
+      <c r="O15" s="12"/>
+      <c r="P15" s="12"/>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="C16" s="20"/>
+      <c r="D16" s="21"/>
+      <c r="F16" s="12"/>
+      <c r="G16" s="12"/>
+      <c r="I16" s="12"/>
+      <c r="J16" s="12"/>
+      <c r="L16" s="12"/>
+      <c r="M16" s="12"/>
+      <c r="O16" s="12"/>
+      <c r="P16" s="12"/>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="C17" s="20"/>
+      <c r="D17" s="21"/>
+      <c r="F17" s="12"/>
+      <c r="G17" s="12"/>
+      <c r="I17" s="12"/>
+      <c r="J17" s="12"/>
+      <c r="L17" s="12"/>
+      <c r="M17" s="12"/>
+      <c r="O17" s="12"/>
+      <c r="P17" s="12"/>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="C18" s="20"/>
+      <c r="D18" s="21"/>
+      <c r="F18" s="12"/>
+      <c r="G18" s="12"/>
+      <c r="I18" s="12"/>
+      <c r="J18" s="12"/>
+      <c r="L18" s="12"/>
+      <c r="M18" s="12"/>
+      <c r="O18" s="12"/>
+      <c r="P18" s="12"/>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="C19" s="23"/>
+      <c r="D19" s="24"/>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="C20" s="25" t="s">
+        <v>93</v>
+      </c>
+      <c r="D20" s="11" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="C21" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="D21" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="F21" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="G21" s="11" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="C22" s="25">
+        <f>F2</f>
+        <v>522.04683333333321</v>
+      </c>
+      <c r="D22" s="25">
+        <f>F1</f>
+        <v>1000</v>
+      </c>
+      <c r="F22" s="25">
+        <f>FORECAST(C22,$D$22:$D$28,$C$22:$C$28)</f>
+        <v>1002.1630725649882</v>
+      </c>
+      <c r="G22" s="25">
+        <f>D22-FORECAST(C22,$D$22:$D$28,$C$22:$C$28)</f>
+        <v>-2.1630725649881697</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="C23" s="25">
+        <f>I2</f>
+        <v>53.739000000000004</v>
+      </c>
+      <c r="D23" s="25">
+        <f>I1</f>
+        <v>500</v>
+      </c>
+      <c r="F23" s="25">
+        <f>FORECAST(C23,$D$22:$D$28,$C$22:$C$28)</f>
+        <v>495.34704578588975</v>
+      </c>
+      <c r="G23" s="25">
+        <f t="shared" ref="G23:G25" si="0">D23-FORECAST(C23,$D$22:$D$28,$C$22:$C$28)</f>
+        <v>4.6529542141102525</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="C24" s="25">
+        <f>L2</f>
+        <v>-172.47499999999997</v>
+      </c>
+      <c r="D24" s="25">
+        <f>L1</f>
+        <v>250</v>
+      </c>
+      <c r="F24" s="25">
+        <f>FORECAST(C24,$D$22:$D$28,$C$22:$C$28)</f>
+        <v>250.53183553036979</v>
+      </c>
+      <c r="G24" s="25">
+        <f t="shared" si="0"/>
+        <v>-0.53183553036978992</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="C25" s="25">
+        <f>O2</f>
+        <v>-402.16200000000009</v>
+      </c>
+      <c r="D25" s="25">
+        <f>O1</f>
+        <v>0</v>
+      </c>
+      <c r="F25" s="25">
+        <f>FORECAST(C25,$D$22:$D$28,$C$22:$C$28)</f>
+        <v>1.958046118752236</v>
+      </c>
+      <c r="G25" s="25">
+        <f t="shared" si="0"/>
+        <v>-1.958046118752236</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="B29" s="11" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A30" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="B30" s="23">
+        <v>1</v>
+      </c>
+      <c r="C30" s="18" t="s">
+        <v>98</v>
+      </c>
+      <c r="D30" s="26">
+        <f>SLOPE($D$22:$D$28,$C$22:$C$28)</f>
+        <v>1.0822283777994288</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A31" s="18" t="s">
+        <v>92</v>
+      </c>
+      <c r="B31" s="23">
+        <v>0</v>
+      </c>
+      <c r="C31" s="18" t="s">
+        <v>99</v>
+      </c>
+      <c r="D31" s="26">
+        <f>D33/1000</f>
+        <v>0.43718917499132626</v>
+      </c>
+      <c r="E31" s="11" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="33" spans="3:16" x14ac:dyDescent="0.2">
+      <c r="C33" s="18" t="s">
+        <v>99</v>
+      </c>
+      <c r="D33" s="23">
+        <f>INTERCEPT($D$22:$D$28,$C$22:$C$28)</f>
+        <v>437.18917499132624</v>
+      </c>
+      <c r="E33" s="11" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="36" spans="3:16" x14ac:dyDescent="0.2">
+      <c r="C36" s="18"/>
+    </row>
+    <row r="37" spans="3:16" x14ac:dyDescent="0.2">
+      <c r="C37" s="18"/>
+    </row>
+    <row r="43" spans="3:16" x14ac:dyDescent="0.2">
+      <c r="F43" s="13">
+        <f>F45*1000</f>
+        <v>1004.9304999999999</v>
+      </c>
+      <c r="G43" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="I43" s="13" t="e">
+        <f>I45*1000</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J43" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="L43" s="13">
+        <f>L45*1000</f>
+        <v>253.67933333333332</v>
+      </c>
+      <c r="M43" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="O43" s="13" t="e">
+        <f>O45*1000</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P43" s="11" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="44" spans="3:16" x14ac:dyDescent="0.2">
+      <c r="F44" s="14">
+        <f>F$1/F43</f>
+        <v>0.99509369055870034</v>
+      </c>
+      <c r="I44" s="14" t="e">
+        <f>I$1/I43</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L44" s="14">
+        <f>L$1/L43</f>
+        <v>0.98549612502923645</v>
+      </c>
+    </row>
+    <row r="45" spans="3:16" x14ac:dyDescent="0.2">
+      <c r="F45" s="15">
+        <f>AVERAGE(F50:F59)</f>
+        <v>1.0049304999999999</v>
+      </c>
+      <c r="G45" s="16">
+        <f>AVERAGE(G50:G59)</f>
+        <v>22.433615000000003</v>
+      </c>
+      <c r="I45" s="15" t="e">
+        <f>AVERAGE(I50:I59)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J45" s="16" t="e">
+        <f>AVERAGE(J50:J59)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L45" s="15">
+        <f>AVERAGE(L50:L59)</f>
+        <v>0.25367933333333331</v>
+      </c>
+      <c r="M45" s="16">
+        <f>AVERAGE(M50:M59)</f>
+        <v>22.24109</v>
+      </c>
+      <c r="O45" s="15" t="e">
+        <f>AVERAGE(O50:O59)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P45" s="16" t="e">
+        <f>AVERAGE(P50:P59)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="46" spans="3:16" x14ac:dyDescent="0.2">
+      <c r="F46" s="15">
+        <f>STDEV(F50:F59)</f>
+        <v>2.7641816148728118E-4</v>
+      </c>
+      <c r="G46" s="16">
+        <f>STDEV(G50:G59)</f>
+        <v>9.5600331240711083E-3</v>
+      </c>
+      <c r="I46" s="15" t="e">
+        <f>STDEV(I50:I59)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J46" s="16" t="e">
+        <f>STDEV(J50:J59)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L46" s="15">
+        <f>STDEV(L50:L59)</f>
+        <v>1.5049539306348826E-3</v>
+      </c>
+      <c r="M46" s="16">
+        <f>STDEV(M50:M59)</f>
+        <v>2.1495178529148156E-2</v>
+      </c>
+      <c r="O46" s="15" t="e">
+        <f>STDEV(O50:O59)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P46" s="16" t="e">
+        <f>STDEV(P50:P59)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="47" spans="3:16" x14ac:dyDescent="0.2">
+      <c r="F47" s="17">
+        <f>F46/F45</f>
+        <v>2.7506196845182947E-4</v>
+      </c>
+      <c r="G47" s="17">
+        <f>G46/G45</f>
+        <v>4.2614768614292019E-4</v>
+      </c>
+      <c r="I47" s="17" t="e">
+        <f>I46/I45</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J47" s="17" t="e">
+        <f>J46/J45</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L47" s="17">
+        <f>L46/L45</f>
+        <v>5.9325050679527808E-3</v>
+      </c>
+      <c r="M47" s="17">
+        <f>M46/M45</f>
+        <v>9.664624588609711E-4</v>
+      </c>
+      <c r="O47" s="17" t="e">
+        <f>O46/O45</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P47" s="17" t="e">
+        <f>P46/P45</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="48" spans="3:16" x14ac:dyDescent="0.2">
+      <c r="F48" s="17"/>
+      <c r="G48" s="17"/>
+      <c r="I48" s="17"/>
+      <c r="J48" s="17"/>
+      <c r="L48" s="17"/>
+      <c r="M48" s="17"/>
+      <c r="O48" s="17"/>
+      <c r="P48" s="17"/>
+    </row>
+    <row r="50" spans="6:16" x14ac:dyDescent="0.2">
+      <c r="F50" s="12">
+        <v>1.004626</v>
+      </c>
+      <c r="G50" s="12">
+        <v>22.440580000000001</v>
+      </c>
+      <c r="I50" s="12"/>
+      <c r="J50" s="12"/>
+      <c r="L50" s="12">
+        <v>0.25512200000000002</v>
+      </c>
+      <c r="M50" s="12">
+        <v>22.228059999999999</v>
+      </c>
+      <c r="O50" s="12"/>
+      <c r="P50" s="12"/>
+    </row>
+    <row r="51" spans="6:16" x14ac:dyDescent="0.2">
+      <c r="F51" s="12">
+        <v>1.0048090000000001</v>
+      </c>
+      <c r="G51" s="12">
+        <v>22.440580000000001</v>
+      </c>
+      <c r="I51" s="12"/>
+      <c r="J51" s="12"/>
+      <c r="L51" s="12">
+        <v>0.25379699999999999</v>
+      </c>
+      <c r="M51" s="12">
+        <v>22.229310000000002</v>
+      </c>
+      <c r="O51" s="12"/>
+      <c r="P51" s="12"/>
+    </row>
+    <row r="52" spans="6:16" x14ac:dyDescent="0.2">
+      <c r="F52" s="12">
+        <v>1.0050190000000001</v>
+      </c>
+      <c r="G52" s="12">
+        <v>22.432980000000001</v>
+      </c>
+      <c r="I52" s="12"/>
+      <c r="J52" s="12"/>
+      <c r="L52" s="12">
+        <v>0.25211899999999998</v>
+      </c>
+      <c r="M52" s="12">
+        <v>22.265899999999998</v>
+      </c>
+      <c r="O52" s="12"/>
+      <c r="P52" s="12"/>
+    </row>
+    <row r="53" spans="6:16" x14ac:dyDescent="0.2">
+      <c r="F53" s="12">
+        <v>1.0052680000000001</v>
+      </c>
+      <c r="G53" s="12">
+        <v>22.42032</v>
+      </c>
+      <c r="I53" s="12"/>
+      <c r="J53" s="12"/>
+      <c r="L53" s="12"/>
+      <c r="M53" s="12"/>
+      <c r="O53" s="12"/>
+      <c r="P53" s="12"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M94"/>
+  <dimension ref="M4:P23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2:J3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O38" sqref="O38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="J1" t="s">
+    <row r="4" spans="13:16" ht="19" x14ac:dyDescent="0.25">
+      <c r="N4" s="7" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="5" spans="13:16" x14ac:dyDescent="0.2">
+      <c r="M5" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="N5">
+        <f>AVERAGE(N8:N19)</f>
+        <v>4.7173500000000006</v>
+      </c>
+      <c r="O5">
+        <f t="shared" ref="O5:P5" si="0">AVERAGE(O8:O19)</f>
+        <v>184.61249000000001</v>
+      </c>
+      <c r="P5">
+        <f>AVERAGE(P8:P19)</f>
+        <v>21.256374000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="13:16" x14ac:dyDescent="0.2">
+      <c r="M6" s="9" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="7" spans="13:16" x14ac:dyDescent="0.2">
+      <c r="M7" s="9"/>
+    </row>
+    <row r="8" spans="13:16" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="M8" s="10"/>
+      <c r="N8" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="O8" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="P8" s="6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="13:16" x14ac:dyDescent="0.2">
+      <c r="M9" s="9"/>
+      <c r="N9" s="8">
+        <v>4.7158769999999999</v>
+      </c>
+      <c r="O9" s="8">
+        <v>184.74780000000001</v>
+      </c>
+      <c r="P9" s="8">
+        <v>21.323270000000001</v>
+      </c>
+    </row>
+    <row r="10" spans="13:16" x14ac:dyDescent="0.2">
+      <c r="M10" s="9"/>
+      <c r="N10" s="8">
+        <v>4.7152289999999999</v>
+      </c>
+      <c r="O10" s="8">
+        <v>184.77850000000001</v>
+      </c>
+      <c r="P10" s="8">
+        <v>21.308250000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="13:16" x14ac:dyDescent="0.2">
+      <c r="M11" s="9"/>
+      <c r="N11" s="8">
+        <v>4.7144339999999998</v>
+      </c>
+      <c r="O11" s="8">
+        <v>184.81700000000001</v>
+      </c>
+      <c r="P11" s="8">
+        <v>21.291409999999999</v>
+      </c>
+    </row>
+    <row r="12" spans="13:16" x14ac:dyDescent="0.2">
+      <c r="M12" s="9"/>
+      <c r="N12" s="8">
+        <v>4.7173749999999997</v>
+      </c>
+      <c r="O12" s="8">
+        <v>184.64019999999999</v>
+      </c>
+      <c r="P12" s="8">
+        <v>21.277280000000001</v>
+      </c>
+    </row>
+    <row r="13" spans="13:16" x14ac:dyDescent="0.2">
+      <c r="M13" s="9"/>
+      <c r="N13" s="8">
+        <v>4.717117</v>
+      </c>
+      <c r="O13" s="8">
+        <v>184.64789999999999</v>
+      </c>
+      <c r="P13" s="8">
+        <v>21.261320000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="13:16" x14ac:dyDescent="0.2">
+      <c r="M14" s="9"/>
+      <c r="N14" s="8">
+        <v>4.7179409999999997</v>
+      </c>
+      <c r="O14" s="8">
+        <v>184.59399999999999</v>
+      </c>
+      <c r="P14" s="8">
+        <v>21.247800000000002</v>
+      </c>
+    </row>
+    <row r="15" spans="13:16" x14ac:dyDescent="0.2">
+      <c r="M15" s="9"/>
+      <c r="N15" s="8">
+        <v>4.7188730000000003</v>
+      </c>
+      <c r="O15" s="8">
+        <v>184.5325</v>
+      </c>
+      <c r="P15" s="8">
+        <v>21.231259999999999</v>
+      </c>
+    </row>
+    <row r="16" spans="13:16" x14ac:dyDescent="0.2">
+      <c r="M16" s="9"/>
+      <c r="N16" s="8">
+        <v>4.718648</v>
+      </c>
+      <c r="O16" s="8">
+        <v>184.5402</v>
+      </c>
+      <c r="P16" s="8">
+        <v>21.219539999999999</v>
+      </c>
+    </row>
+    <row r="17" spans="13:16" x14ac:dyDescent="0.2">
+      <c r="M17" s="9"/>
+      <c r="N17" s="8">
+        <v>4.7183270000000004</v>
+      </c>
+      <c r="O17" s="8">
+        <v>184.43260000000001</v>
+      </c>
+      <c r="P17" s="8">
+        <v>21.205100000000002</v>
+      </c>
+    </row>
+    <row r="18" spans="13:16" x14ac:dyDescent="0.2">
+      <c r="M18" s="9"/>
+      <c r="N18" s="8">
+        <v>4.7196790000000002</v>
+      </c>
+      <c r="O18" s="8">
+        <v>184.39420000000001</v>
+      </c>
+      <c r="P18" s="8">
+        <v>21.198509999999999</v>
+      </c>
+    </row>
+    <row r="19" spans="13:16" x14ac:dyDescent="0.2">
+      <c r="M19" s="9"/>
+    </row>
+    <row r="20" spans="13:16" x14ac:dyDescent="0.2">
+      <c r="M20" s="9"/>
+    </row>
+    <row r="21" spans="13:16" x14ac:dyDescent="0.2">
+      <c r="M21" s="9"/>
+      <c r="N21" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="13:16" x14ac:dyDescent="0.2">
+      <c r="M22" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="N22">
+        <v>60.609789999999997</v>
+      </c>
+      <c r="O22">
+        <v>52.395429999999998</v>
+      </c>
+      <c r="P22">
+        <v>-0.48604000000000003</v>
+      </c>
+    </row>
+    <row r="23" spans="13:16" x14ac:dyDescent="0.2">
+      <c r="M23" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="N23">
+        <v>60.609789999999997</v>
+      </c>
+      <c r="O23">
+        <v>52.521470000000001</v>
+      </c>
+      <c r="P23">
+        <v>-1.3863239999999999</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3F6F1C1-5893-E147-BDD3-36630E191997}">
+  <dimension ref="A1:D94"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F26" sqref="F26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="B5" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="B6" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="B7" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="B8" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="B9" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="B10" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="B11" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="B12" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D12" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>1</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" s="2">
+        <v>1342.86</v>
+      </c>
+      <c r="D13" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>2</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C14" s="2">
+        <v>285.70999999999998</v>
+      </c>
+      <c r="D14" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>3</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C15" s="2">
+        <v>228.57</v>
+      </c>
+      <c r="D15" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>4</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C16" s="2">
+        <v>171.43</v>
+      </c>
+      <c r="D16" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>5</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C17" s="2">
+        <v>114.29</v>
+      </c>
+      <c r="D17" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>6</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C18" s="2">
+        <v>57.14</v>
+      </c>
+      <c r="D18" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>7</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C19" s="2">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
+      <c r="D19" t="s">
         <v>1</v>
       </c>
-      <c r="C2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F2" t="s">
-        <v>3</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A3">
-        <v>4.7158769999999999</v>
-      </c>
-      <c r="B3">
-        <v>184.74780000000001</v>
-      </c>
-      <c r="C3">
-        <v>21.323270000000001</v>
-      </c>
-      <c r="F3">
-        <v>60.609789999999997</v>
-      </c>
-      <c r="G3">
-        <v>52.395429999999998</v>
-      </c>
-      <c r="H3">
-        <v>-0.48604000000000003</v>
-      </c>
-      <c r="J3" s="4" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A4">
-        <v>4.7152289999999999</v>
-      </c>
-      <c r="B4">
-        <v>184.77850000000001</v>
-      </c>
-      <c r="C4">
-        <v>21.308250000000001</v>
-      </c>
-      <c r="F4">
-        <v>60.609789999999997</v>
-      </c>
-      <c r="G4">
-        <v>52.521470000000001</v>
-      </c>
-      <c r="H4">
-        <v>-1.3863239999999999</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" ht="17" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <v>4.7144339999999998</v>
-      </c>
-      <c r="B5">
-        <v>184.81700000000001</v>
-      </c>
-      <c r="C5">
-        <v>21.291409999999999</v>
-      </c>
-      <c r="K5" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" ht="17" x14ac:dyDescent="0.2">
-      <c r="A6">
-        <v>4.7173749999999997</v>
-      </c>
-      <c r="B6">
-        <v>184.64019999999999</v>
-      </c>
-      <c r="C6">
-        <v>21.277280000000001</v>
-      </c>
-      <c r="K6" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="L6" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" ht="17" x14ac:dyDescent="0.2">
-      <c r="A7">
-        <v>4.717117</v>
-      </c>
-      <c r="B7">
-        <v>184.64789999999999</v>
-      </c>
-      <c r="C7">
-        <v>21.261320000000001</v>
-      </c>
-      <c r="K7" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="L7" s="2" t="s">
+    </row>
+    <row r="20" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A20">
         <v>8</v>
       </c>
-    </row>
-    <row r="8" spans="1:13" ht="17" x14ac:dyDescent="0.2">
-      <c r="A8">
-        <v>4.7179409999999997</v>
-      </c>
-      <c r="B8">
-        <v>184.59399999999999</v>
-      </c>
-      <c r="C8">
-        <v>21.247800000000002</v>
-      </c>
-      <c r="K8" s="2" t="s">
+      <c r="B20" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C20" s="2">
+        <v>-57.14</v>
+      </c>
+      <c r="D20" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A21">
         <v>9</v>
       </c>
-      <c r="L8" s="2" t="s">
+      <c r="B21" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C21" s="2">
+        <v>-114.29</v>
+      </c>
+      <c r="D21" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A22">
         <v>10</v>
       </c>
-    </row>
-    <row r="9" spans="1:13" ht="17" x14ac:dyDescent="0.2">
-      <c r="A9">
-        <v>4.7188730000000003</v>
-      </c>
-      <c r="B9">
-        <v>184.5325</v>
-      </c>
-      <c r="C9">
-        <v>21.231259999999999</v>
-      </c>
-      <c r="K9" s="2" t="s">
+      <c r="B22" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C22" s="2">
+        <v>-171.43</v>
+      </c>
+      <c r="D22" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A23">
         <v>11</v>
       </c>
-      <c r="L9" s="2" t="s">
+      <c r="B23" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C23" s="2">
+        <v>-228.57</v>
+      </c>
+      <c r="D23" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A24">
         <v>12</v>
       </c>
-    </row>
-    <row r="10" spans="1:13" ht="17" x14ac:dyDescent="0.2">
-      <c r="A10">
-        <v>4.718648</v>
-      </c>
-      <c r="B10">
-        <v>184.5402</v>
-      </c>
-      <c r="C10">
-        <v>21.219539999999999</v>
-      </c>
-      <c r="K10" s="1" t="s">
+      <c r="B24" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C24" s="2">
+        <v>-285.70999999999998</v>
+      </c>
+      <c r="D24" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A25">
         <v>13</v>
       </c>
-    </row>
-    <row r="11" spans="1:13" ht="17" x14ac:dyDescent="0.2">
-      <c r="A11">
-        <v>4.7183270000000004</v>
-      </c>
-      <c r="B11">
-        <v>184.43260000000001</v>
-      </c>
-      <c r="C11">
-        <v>21.205100000000002</v>
-      </c>
-      <c r="K11" s="1" t="s">
+      <c r="B25" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C25" s="2">
+        <v>-342.86</v>
+      </c>
+      <c r="D25" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A26">
         <v>14</v>
       </c>
-    </row>
-    <row r="12" spans="1:13" ht="17" x14ac:dyDescent="0.2">
-      <c r="A12">
-        <v>4.7196790000000002</v>
-      </c>
-      <c r="B12">
-        <v>184.39420000000001</v>
-      </c>
-      <c r="C12">
-        <v>21.198509999999999</v>
-      </c>
-      <c r="K12" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="L12" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="M12" t="s">
+      <c r="B26" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C26" s="2">
+        <v>-400</v>
+      </c>
+      <c r="D26" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="17" x14ac:dyDescent="0.2">
-      <c r="J13">
-        <v>1</v>
-      </c>
-      <c r="K13" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="L13" s="2">
-        <v>1342.86</v>
-      </c>
-      <c r="M13" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" ht="17" x14ac:dyDescent="0.2">
-      <c r="J14">
-        <v>2</v>
-      </c>
-      <c r="K14" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="L14" s="2">
-        <v>285.70999999999998</v>
-      </c>
-      <c r="M14" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" ht="17" x14ac:dyDescent="0.2">
-      <c r="J15">
-        <v>3</v>
-      </c>
-      <c r="K15" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="L15" s="2">
-        <v>228.57</v>
-      </c>
-      <c r="M15" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" ht="17" x14ac:dyDescent="0.2">
-      <c r="J16">
-        <v>4</v>
-      </c>
-      <c r="K16" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="L16" s="2">
-        <v>171.43</v>
-      </c>
-      <c r="M16" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="10:13" ht="17" x14ac:dyDescent="0.2">
-      <c r="J17">
-        <v>5</v>
-      </c>
-      <c r="K17" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L17" s="2">
-        <v>114.29</v>
-      </c>
-      <c r="M17" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="10:13" ht="17" x14ac:dyDescent="0.2">
-      <c r="J18">
-        <v>6</v>
-      </c>
-      <c r="K18" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="L18" s="2">
-        <v>57.14</v>
-      </c>
-      <c r="M18" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="10:13" ht="17" x14ac:dyDescent="0.2">
-      <c r="J19">
-        <v>7</v>
-      </c>
-      <c r="K19" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="L19" s="2">
-        <v>0</v>
-      </c>
-      <c r="M19" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="10:13" ht="17" x14ac:dyDescent="0.2">
-      <c r="J20">
-        <v>8</v>
-      </c>
-      <c r="K20" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="L20" s="2">
-        <v>-57.14</v>
-      </c>
-      <c r="M20" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="10:13" ht="17" x14ac:dyDescent="0.2">
-      <c r="J21">
-        <v>9</v>
-      </c>
-      <c r="K21" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="L21" s="2">
-        <v>-114.29</v>
-      </c>
-      <c r="M21" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="10:13" ht="17" x14ac:dyDescent="0.2">
-      <c r="J22">
-        <v>10</v>
-      </c>
-      <c r="K22" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="L22" s="2">
-        <v>-171.43</v>
-      </c>
-      <c r="M22" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="10:13" ht="17" x14ac:dyDescent="0.2">
-      <c r="J23">
-        <v>11</v>
-      </c>
-      <c r="K23" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="L23" s="2">
-        <v>-228.57</v>
-      </c>
-      <c r="M23" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="10:13" ht="17" x14ac:dyDescent="0.2">
-      <c r="J24">
-        <v>12</v>
-      </c>
-      <c r="K24" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="L24" s="2">
-        <v>-285.70999999999998</v>
-      </c>
-      <c r="M24" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="10:13" ht="17" x14ac:dyDescent="0.2">
-      <c r="J25">
-        <v>13</v>
-      </c>
-      <c r="K25" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="L25" s="2">
-        <v>-342.86</v>
-      </c>
-      <c r="M25" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="10:13" ht="17" x14ac:dyDescent="0.2">
-      <c r="J26">
-        <v>14</v>
-      </c>
-      <c r="K26" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="L26" s="2">
-        <v>-400</v>
-      </c>
-      <c r="M26" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="10:13" ht="17" x14ac:dyDescent="0.2">
-      <c r="J29" s="3" t="s">
+    <row r="29" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A29" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="10:13" x14ac:dyDescent="0.2">
-      <c r="J30" s="4" t="s">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30" s="4" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="32" spans="10:13" ht="16" x14ac:dyDescent="0.2">
-      <c r="J32" s="5" t="s">
+    <row r="32" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A32" s="5" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="33" spans="10:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="J33" s="5" t="s">
+    <row r="33" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A33" s="5" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="34" spans="10:10" ht="18" x14ac:dyDescent="0.25">
-      <c r="J34" s="5" t="s">
+    <row r="34" spans="1:1" ht="18" x14ac:dyDescent="0.25">
+      <c r="A34" s="5" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="35" spans="10:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="J35" s="5" t="s">
+    <row r="35" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A35" s="5" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="37" spans="10:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="J37" s="5" t="s">
+    <row r="37" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A37" s="5" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="39" spans="10:10" ht="18" x14ac:dyDescent="0.25">
-      <c r="J39" s="5" t="s">
+    <row r="39" spans="1:1" ht="18" x14ac:dyDescent="0.25">
+      <c r="A39" s="5" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="41" spans="10:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="J41" s="5" t="s">
+    <row r="41" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A41" s="5" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="43" spans="10:10" ht="18" x14ac:dyDescent="0.25">
-      <c r="J43" s="5" t="s">
+    <row r="43" spans="1:1" ht="18" x14ac:dyDescent="0.25">
+      <c r="A43" s="5" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="45" spans="10:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="J45" s="5" t="s">
+    <row r="45" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A45" s="5" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="47" spans="10:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="J47" s="5" t="s">
+    <row r="47" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A47" s="5" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="49" spans="10:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="J49" s="5" t="s">
+    <row r="49" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A49" s="5" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="51" spans="10:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="J51" s="5" t="s">
+    <row r="51" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A51" s="5" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="53" spans="10:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="J53" s="5" t="s">
+    <row r="53" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A53" s="5" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="55" spans="10:10" ht="18" x14ac:dyDescent="0.25">
-      <c r="J55" s="5" t="s">
+    <row r="55" spans="1:1" ht="18" x14ac:dyDescent="0.25">
+      <c r="A55" s="5" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="57" spans="10:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="J57" s="5" t="s">
+    <row r="57" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A57" s="5" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="59" spans="10:10" ht="18" x14ac:dyDescent="0.25">
-      <c r="J59" s="5" t="s">
+    <row r="59" spans="1:1" ht="18" x14ac:dyDescent="0.25">
+      <c r="A59" s="5" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="61" spans="10:10" ht="18" x14ac:dyDescent="0.25">
-      <c r="J61" s="5" t="s">
+    <row r="61" spans="1:1" ht="18" x14ac:dyDescent="0.25">
+      <c r="A61" s="5" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="62" spans="10:10" ht="18" x14ac:dyDescent="0.25">
-      <c r="J62" s="5" t="s">
+    <row r="62" spans="1:1" ht="18" x14ac:dyDescent="0.25">
+      <c r="A62" s="5" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="63" spans="10:10" ht="18" x14ac:dyDescent="0.2">
-      <c r="J63" s="5" t="s">
+    <row r="63" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A63" s="5" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="64" spans="10:10" ht="18" x14ac:dyDescent="0.2">
-      <c r="J64" s="5" t="s">
+    <row r="64" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A64" s="5" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="65" spans="10:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="J65" s="5" t="s">
+    <row r="65" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A65" s="5" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="67" spans="10:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="J67" s="5" t="s">
+    <row r="67" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A67" s="5" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="69" spans="10:10" ht="18" x14ac:dyDescent="0.25">
-      <c r="J69" s="5" t="s">
+    <row r="69" spans="1:1" ht="18" x14ac:dyDescent="0.25">
+      <c r="A69" s="5" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="70" spans="10:10" ht="18" x14ac:dyDescent="0.25">
-      <c r="J70" s="5" t="s">
+    <row r="70" spans="1:1" ht="18" x14ac:dyDescent="0.25">
+      <c r="A70" s="5" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="72" spans="10:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="J72" s="5" t="s">
+    <row r="72" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A72" s="5" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="73" spans="10:10" ht="18" x14ac:dyDescent="0.25">
-      <c r="J73" s="5" t="s">
+    <row r="73" spans="1:1" ht="18" x14ac:dyDescent="0.25">
+      <c r="A73" s="5" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="74" spans="10:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="J74" s="5" t="s">
+    <row r="74" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A74" s="5" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="75" spans="10:10" ht="18" x14ac:dyDescent="0.25">
-      <c r="J75" s="5" t="s">
+    <row r="75" spans="1:1" ht="18" x14ac:dyDescent="0.25">
+      <c r="A75" s="5" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="77" spans="10:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="J77" s="5" t="s">
+    <row r="77" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A77" s="5" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="79" spans="10:10" ht="18" x14ac:dyDescent="0.25">
-      <c r="J79" s="5" t="s">
+    <row r="79" spans="1:1" ht="18" x14ac:dyDescent="0.25">
+      <c r="A79" s="5" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="80" spans="10:10" ht="18" x14ac:dyDescent="0.25">
-      <c r="J80" s="5" t="s">
+    <row r="80" spans="1:1" ht="18" x14ac:dyDescent="0.25">
+      <c r="A80" s="5" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="82" spans="10:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="J82" s="5" t="s">
+    <row r="82" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A82" s="5" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="84" spans="10:10" ht="18" x14ac:dyDescent="0.25">
-      <c r="J84" s="5" t="s">
+    <row r="84" spans="1:1" ht="18" x14ac:dyDescent="0.25">
+      <c r="A84" s="5" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="86" spans="10:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="J86" s="5" t="s">
+    <row r="86" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A86" s="5" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="88" spans="10:10" ht="18" x14ac:dyDescent="0.25">
-      <c r="J88" s="5" t="s">
+    <row r="88" spans="1:1" ht="18" x14ac:dyDescent="0.25">
+      <c r="A88" s="5" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="90" spans="10:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="J90" s="5" t="s">
+    <row r="90" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A90" s="5" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="92" spans="10:10" ht="18" x14ac:dyDescent="0.25">
-      <c r="J92" s="5" t="s">
+    <row r="92" spans="1:1" ht="18" x14ac:dyDescent="0.25">
+      <c r="A92" s="5" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="94" spans="10:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="J94" s="5" t="s">
+    <row r="94" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A94" s="5" t="s">
         <v>67</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="J30" r:id="rId1" xr:uid="{4BDC9DF2-BB79-4246-8E93-9D366A393AB5}"/>
-    <hyperlink ref="J32" r:id="rId2" display="http://en.wikipedia.org/wiki/Instrumentation_amplifier" xr:uid="{D5BD5E1A-656A-6740-9507-E152A6D793C6}"/>
-    <hyperlink ref="J2" r:id="rId3" xr:uid="{219E1F00-04EB-FC40-9FC2-283CB79C695F}"/>
-    <hyperlink ref="J3" r:id="rId4" xr:uid="{757A8F35-7AFB-884D-B939-B2CFD7E90FCC}"/>
+    <hyperlink ref="A30" r:id="rId1" xr:uid="{E967285A-3B98-504F-BB84-C1B39D81C4A5}"/>
+    <hyperlink ref="A32" r:id="rId2" display="http://en.wikipedia.org/wiki/Instrumentation_amplifier" xr:uid="{81E0FEAC-C6C3-7E4E-AC08-28FA021AD8B8}"/>
+    <hyperlink ref="A2" r:id="rId3" xr:uid="{05F083E4-FBCD-1240-9F60-80F1C34E0F6C}"/>
+    <hyperlink ref="A3" r:id="rId4" xr:uid="{8A3E71AA-ECF8-374F-8EAB-2BC21FEA21B6}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId5"/>

</xml_diff>